<commit_message>
Make fixture more complex
</commit_message>
<xml_diff>
--- a/test/fixtures/merged.xlsx
+++ b/test/fixtures/merged.xlsx
@@ -32,11 +32,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="15">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -54,51 +55,85 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -199,29 +234,61 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,10 +385,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,6 +401,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
+      <c r="C1" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -346,9 +416,29 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>